<commit_message>
Dev Swordlake 4 the
</commit_message>
<xml_diff>
--- a/TDH-WEP-1.xlsx
+++ b/TDH-WEP-1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macosx/Desktop/WEP/Tự Động Hoá/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arduino\WE-TTTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14505" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Saw" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -249,8 +249,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +300,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,8 +366,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -448,13 +496,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -489,12 +571,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -505,16 +581,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
+    <cellStyle name="Accent2" xfId="6" builtinId="33"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,7 +742,7 @@
         <xdr:cNvPr id="2" name="Hình ảnh 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{139B7F3F-4ADB-403D-986E-8F1D35B15F2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{139B7F3F-4ADB-403D-986E-8F1D35B15F2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -703,7 +803,7 @@
         <xdr:cNvPr id="3" name="Hình ảnh 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143A7FF0-DBDB-4F76-9691-7E9E276E2E44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143A7FF0-DBDB-4F76-9691-7E9E276E2E44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -764,7 +864,7 @@
         <xdr:cNvPr id="4" name="Hình ảnh 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB051C85-CEBB-41A4-ADDF-B919EB17F52D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB051C85-CEBB-41A4-ADDF-B919EB17F52D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1103,12 +1203,12 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="35.1640625" customWidth="1"/>
+    <col min="2" max="4" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1243,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1190,16 +1290,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="4" width="27.1640625" customWidth="1"/>
+    <col min="2" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -1213,75 +1313,76 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+    <row r="2" spans="1:5" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="150" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+    <row r="5" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+    <row r="6" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1298,12 +1399,12 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="34.1640625" customWidth="1"/>
+    <col min="1" max="4" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1439,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1352,7 +1453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1366,7 +1467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1380,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1394,7 +1495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1408,12 +1509,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>20</v>
       </c>
@@ -1428,16 +1529,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1451,81 +1552,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+    <row r="4" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1539,21 +1640,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
     </row>
   </sheetData>
@@ -1566,15 +1667,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="23.6640625" customWidth="1"/>
+    <col min="1" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1588,21 +1689,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1616,7 +1717,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1630,7 +1731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1644,7 +1745,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1658,32 +1759,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1697,16 +1798,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="4" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -1720,7 +1821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>